<commit_message>
replaced cilck play button with image recog
</commit_message>
<xml_diff>
--- a/Generate Build CommandLine.xlsx
+++ b/Generate Build CommandLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Desktop\builderBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83BC854C-876A-4AF8-AEF4-216AF401CC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185B715D-C43C-49DB-B2D3-DE831233E853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2805" yWindow="4215" windowWidth="28800" windowHeight="15435" xr2:uid="{BABD2F72-0E3F-40ED-8E50-B1C2AD414C40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="16">
   <si>
     <t>','C:\\Users\\Nicky\\Desktop\\builderBase\\assets\\</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve"> --add-data="assets\</t>
+  </si>
+  <si>
+    <t>play.png</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D68544B-DDBB-4203-99A3-AFF33270D1EA}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,9 +771,24 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
       <c r="E24" t="str">
-        <f>_xlfn.CONCAT(E23," builderBase.py")</f>
-        <v>pyinstaller --onefile --add-data="assets\attack.png;assets" --add-data="assets\attack2.png;assets" --add-data="assets\collect.png;assets" --add-data="assets\elixirBase.png;assets" --add-data="assets\elixirElixir.png;assets" --add-data="assets\elixirFight.png;assets" --add-data="assets\findnow.png;assets" --add-data="assets\secondClean.png;assets" --add-data="assets\secondDirty.png;assets" builderBase.py</v>
+        <f t="shared" ref="E24" si="2">_xlfn.CONCAT(E23,B24,C24,D24)</f>
+        <v>pyinstaller --onefile --add-data="assets\attack.png;assets" --add-data="assets\attack2.png;assets" --add-data="assets\collect.png;assets" --add-data="assets\elixirBase.png;assets" --add-data="assets\elixirElixir.png;assets" --add-data="assets\elixirFight.png;assets" --add-data="assets\findnow.png;assets" --add-data="assets\secondClean.png;assets" --add-data="assets\secondDirty.png;assets" --add-data="assets\play.png;assets"</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="str">
+        <f>_xlfn.CONCAT(E24," builderBase.py")</f>
+        <v>pyinstaller --onefile --add-data="assets\attack.png;assets" --add-data="assets\attack2.png;assets" --add-data="assets\collect.png;assets" --add-data="assets\elixirBase.png;assets" --add-data="assets\elixirElixir.png;assets" --add-data="assets\elixirFight.png;assets" --add-data="assets\findnow.png;assets" --add-data="assets\secondClean.png;assets" --add-data="assets\secondDirty.png;assets" --add-data="assets\play.png;assets" builderBase.py</v>
       </c>
     </row>
   </sheetData>

</xml_diff>